<commit_message>
some sql views and stuff
</commit_message>
<xml_diff>
--- a/doc/Analyse.xlsx
+++ b/doc/Analyse.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Gruppe A</t>
   </si>
@@ -37,6 +37,75 @@
   </si>
   <si>
     <t>AnalysisTime manchmal 0 =&gt; Keine Erkenntnisse über OK oder NOK</t>
+  </si>
+  <si>
+    <t>Material Numbers</t>
+  </si>
+  <si>
+    <t>OK Percentage</t>
+  </si>
+  <si>
+    <t>0.796536796536797</t>
+  </si>
+  <si>
+    <t>0.946351931330472</t>
+  </si>
+  <si>
+    <t>Gruppe</t>
+  </si>
+  <si>
+    <t>Material Number</t>
+  </si>
+  <si>
+    <t>0.932432432432432</t>
+  </si>
+  <si>
+    <t>0.953125</t>
+  </si>
+  <si>
+    <t>0.957894736842105</t>
+  </si>
+  <si>
+    <t>0.951219512195122</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>0.975308641975309</t>
+  </si>
+  <si>
+    <t>0.779411764705882</t>
+  </si>
+  <si>
+    <t>0.742268041237113</t>
+  </si>
+  <si>
+    <t>0.753424657534247</t>
+  </si>
+  <si>
+    <t>0.81578947368421</t>
+  </si>
+  <si>
+    <t>0.810126582278481</t>
+  </si>
+  <si>
+    <t>0.898550724637681</t>
+  </si>
+  <si>
+    <t>MinAnalysisTime</t>
+  </si>
+  <si>
+    <t>AvgAnalysisTime</t>
+  </si>
+  <si>
+    <t>MaxAnalysisTime</t>
+  </si>
+  <si>
+    <t>MinMillingHeat</t>
+  </si>
+  <si>
+    <t>AvgMillingHeat</t>
   </si>
 </sst>
 </file>
@@ -189,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -209,6 +278,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -219,14 +295,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -264,9 +343,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -301,7 +380,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -336,7 +415,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -510,23 +589,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M34"/>
+  <dimension ref="A2:AC51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.5703125" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
     <col min="13" max="13" width="59.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,11 +655,72 @@
       <c r="G3" s="3">
         <v>7432</v>
       </c>
-      <c r="M3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="17"/>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>8822.2038626609501</v>
+      </c>
+      <c r="L3">
+        <v>19016</v>
+      </c>
+      <c r="M3">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="N3">
+        <v>114.709047925608</v>
+      </c>
+      <c r="O3">
+        <v>170.58</v>
+      </c>
+      <c r="P3">
+        <v>100</v>
+      </c>
+      <c r="Q3">
+        <v>129.29902274678099</v>
+      </c>
+      <c r="R3">
+        <v>170.58</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>7116.6666666666697</v>
+      </c>
+      <c r="U3">
+        <v>11500</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>8753.3333333333303</v>
+      </c>
+      <c r="X3">
+        <v>14980</v>
+      </c>
+      <c r="Y3">
+        <v>20013</v>
+      </c>
+      <c r="Z3">
+        <v>20036.8626609442</v>
+      </c>
+      <c r="AA3">
+        <v>20627</v>
+      </c>
+      <c r="AB3">
+        <v>17005</v>
+      </c>
+      <c r="AC3">
+        <v>17031.263948497901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
@@ -574,172 +742,386 @@
       <c r="G4" s="9">
         <v>9823</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2" t="s">
+      <c r="H4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="17"/>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>9457.0173160173199</v>
+      </c>
+      <c r="L4">
+        <v>19015</v>
+      </c>
+      <c r="M4">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="N4">
+        <v>157.188378787879</v>
+      </c>
+      <c r="O4">
+        <v>240.93</v>
+      </c>
+      <c r="P4">
+        <v>120</v>
+      </c>
+      <c r="Q4">
+        <v>234.992209090909</v>
+      </c>
+      <c r="R4">
+        <v>324.93</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>9160</v>
+      </c>
+      <c r="U4">
+        <v>15000</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>11333.333333333299</v>
+      </c>
+      <c r="X4">
+        <v>18500</v>
+      </c>
+      <c r="Y4">
+        <v>27014</v>
+      </c>
+      <c r="Z4">
+        <v>27039.508658008701</v>
+      </c>
+      <c r="AA4">
+        <v>27685</v>
+      </c>
+      <c r="AB4">
+        <v>24012</v>
+      </c>
+      <c r="AC4">
+        <v>24034</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>4248</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>5653</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>6443</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>7134</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>7423</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>7432</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>7742</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>8235</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>8354</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>8414</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>8932</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>9823</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2" t="s">
+      <c r="D36" s="2"/>
+      <c r="E36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F36" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="5">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="5">
         <v>11280</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5">
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5">
         <v>9850</v>
       </c>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5">
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5">
         <v>11</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="6">
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="6">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="5">
         <v>14980</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5">
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5">
         <v>11500</v>
       </c>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5">
+      <c r="F39" s="6"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5">
         <v>6</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="6">
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="6">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5">
-        <v>0</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5">
-        <v>0</v>
-      </c>
-      <c r="F24" s="6"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="5">
+        <v>0</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5">
+        <v>0</v>
+      </c>
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="6"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B43" s="5">
         <v>15500</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5">
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5">
         <v>12480</v>
       </c>
-      <c r="F26" s="6"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5">
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5">
         <v>14</v>
       </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="6">
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="6">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="5">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="5">
         <v>18500</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5">
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5">
         <v>15000</v>
       </c>
-      <c r="F28" s="6"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5">
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5">
         <v>10</v>
       </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="6">
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="6">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
-      <c r="B30" s="8">
-        <v>0</v>
-      </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8">
-        <v>0</v>
-      </c>
-      <c r="F30" s="9"/>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="s">
+    <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="7"/>
+      <c r="B47" s="8">
+        <v>0</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8">
+        <v>0</v>
+      </c>
+      <c r="F47" s="9"/>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="12"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A34:F34"/>
+  <mergeCells count="2">
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="B2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>